<commit_message>
update: model extensions (including updated excel sample)
</commit_message>
<xml_diff>
--- a/ShippingMark/wwwroot/example_excel/upload_template.xlsx
+++ b/ShippingMark/wwwroot/example_excel/upload_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vogia\Documents\GitHub\ShippingMark\ShippingMark\wwwroot\example_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A137EC64-D5C0-4465-894C-833D6A8C36E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD166C18-E8F2-4112-A61F-9A907C19AB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9FB053E7-4228-4295-9A09-A22C30AC7F5C}"/>
+    <workbookView xWindow="-75" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{9FB053E7-4228-4295-9A09-A22C30AC7F5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="101">
   <si>
     <t>CARTON NO</t>
   </si>
@@ -286,6 +286,57 @@
   </si>
   <si>
     <t>2XL</t>
+  </si>
+  <si>
+    <t>000</t>
+  </si>
+  <si>
+    <t>2XS</t>
+  </si>
+  <si>
+    <t>3XL</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>X2</t>
+  </si>
+  <si>
+    <t>X3</t>
+  </si>
+  <si>
+    <t>LL</t>
+  </si>
+  <si>
+    <t>L3</t>
+  </si>
+  <si>
+    <t>L4</t>
+  </si>
+  <si>
+    <t>L5</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>60</t>
   </si>
 </sst>
 </file>
@@ -396,13 +447,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -459,11 +511,15 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{DB61BEF1-50FC-4A49-8CDF-9DB54297BFF3}"/>
+    <cellStyle name="Normal 3" xfId="4" xr:uid="{CBD62CC7-C409-4FEA-B93D-54E1C804ADA7}"/>
     <cellStyle name="표준_HSI0210100K LBS07248459 - 5000 PCS  송하,신성(대우)(LB5908) (638) A " xfId="3" xr:uid="{2EF08E0A-2701-4E3F-85AE-3465AA0DF346}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -480,9 +536,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -520,7 +576,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -626,7 +682,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -768,7 +824,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -776,44 +832,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{555263AD-5947-4833-A0AF-64316F79D6BC}">
-  <dimension ref="A1:BZ11"/>
+  <dimension ref="A1:CQ11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="CK2" sqref="CK2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="1.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="2.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="3.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="2.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="3.21875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="2.109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.21875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="2.109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="3.21875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="2.109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="67" width="3.21875" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="2" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="2.88671875" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="1.88671875" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="3.109375" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="4.21875" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="76" max="77" width="4.109375" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="3.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.21875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.21875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="3.21875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="67" width="3.21875" bestFit="1" customWidth="1"/>
+    <col min="68" max="73" width="3.21875" customWidth="1"/>
+    <col min="74" max="74" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="3.21875" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="2" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="2.88671875" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="1.88671875" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="4.21875" customWidth="1"/>
+    <col min="82" max="82" width="2.21875" bestFit="1" customWidth="1"/>
+    <col min="83" max="85" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="2.88671875" bestFit="1" customWidth="1"/>
+    <col min="87" max="89" width="3" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" ht="25.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:95" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A1" s="7"/>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -894,8 +958,25 @@
       <c r="BX1" s="7"/>
       <c r="BY1" s="7"/>
       <c r="BZ1" s="7"/>
+      <c r="CA1" s="7"/>
+      <c r="CB1" s="7"/>
+      <c r="CC1" s="7"/>
+      <c r="CD1" s="7"/>
+      <c r="CE1" s="7"/>
+      <c r="CF1" s="7"/>
+      <c r="CG1" s="7"/>
+      <c r="CH1" s="7"/>
+      <c r="CI1" s="7"/>
+      <c r="CJ1" s="7"/>
+      <c r="CK1" s="7"/>
+      <c r="CL1" s="7"/>
+      <c r="CM1" s="7"/>
+      <c r="CN1" s="7"/>
+      <c r="CO1" s="7"/>
+      <c r="CP1" s="7"/>
+      <c r="CQ1" s="7"/>
     </row>
-    <row r="2" spans="1:78" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:95" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
@@ -920,225 +1001,276 @@
       <c r="J2" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="L2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="M2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="N2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="14" t="s">
+      <c r="O2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="14" t="s">
+      <c r="P2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="14" t="s">
+      <c r="Q2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="Q2" s="14" t="s">
+      <c r="R2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="14" t="s">
+      <c r="S2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="S2" s="14" t="s">
+      <c r="T2" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="T2" s="14" t="s">
+      <c r="U2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="U2" s="14" t="s">
+      <c r="V2" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="V2" s="14" t="s">
+      <c r="W2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="W2" s="14" t="s">
+      <c r="X2" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="X2" s="14" t="s">
+      <c r="Y2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="Y2" s="14" t="s">
+      <c r="Z2" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="Z2" s="14" t="s">
+      <c r="AA2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="AA2" s="14" t="s">
+      <c r="AB2" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="AB2" s="14" t="s">
+      <c r="AC2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="AC2" s="14" t="s">
+      <c r="AD2" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="AD2" s="14" t="s">
+      <c r="AE2" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="AE2" s="14" t="s">
+      <c r="AF2" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="AF2" s="14" t="s">
+      <c r="AG2" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="AG2" s="14" t="s">
+      <c r="AH2" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="AH2" s="14" t="s">
+      <c r="AI2" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="AI2" s="14" t="s">
+      <c r="AJ2" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="AJ2" s="14" t="s">
+      <c r="AK2" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="AK2" s="14" t="s">
+      <c r="AL2" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="AL2" s="14" t="s">
+      <c r="AM2" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="AM2" s="14" t="s">
+      <c r="AN2" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="AN2" s="14" t="s">
+      <c r="AO2" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="AO2" s="14" t="s">
+      <c r="AP2" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="AP2" s="14" t="s">
+      <c r="AQ2" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="AQ2" s="14" t="s">
+      <c r="AR2" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="AR2" s="14" t="s">
+      <c r="AS2" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="AS2" s="14" t="s">
+      <c r="AT2" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="AT2" s="14" t="s">
+      <c r="AU2" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="AU2" s="14" t="s">
+      <c r="AV2" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="AV2" s="14" t="s">
+      <c r="AW2" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="AW2" s="14" t="s">
+      <c r="AX2" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="AX2" s="14" t="s">
+      <c r="AY2" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="AY2" s="14" t="s">
+      <c r="AZ2" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="AZ2" s="14" t="s">
+      <c r="BA2" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="BA2" s="14" t="s">
+      <c r="BB2" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="BB2" s="14" t="s">
+      <c r="BC2" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="BC2" s="14" t="s">
+      <c r="BD2" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="BD2" s="14" t="s">
+      <c r="BE2" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="BE2" s="14" t="s">
+      <c r="BF2" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="BF2" s="14" t="s">
+      <c r="BG2" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="BG2" s="14" t="s">
+      <c r="BH2" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="BH2" s="14" t="s">
+      <c r="BI2" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="BI2" s="14" t="s">
+      <c r="BJ2" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="BJ2" s="14" t="s">
+      <c r="BK2" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="BK2" s="14" t="s">
+      <c r="BL2" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="BL2" s="14" t="s">
+      <c r="BM2" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="BM2" s="14" t="s">
+      <c r="BN2" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="BN2" s="14" t="s">
+      <c r="BO2" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="BO2" s="14" t="s">
+      <c r="BP2" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="BQ2" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="BR2" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="BS2" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="BT2" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="BU2" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="BV2" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="BW2" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="BP2" s="14" t="s">
+      <c r="BX2" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="BQ2" s="14" t="s">
+      <c r="BY2" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="BR2" s="14" t="s">
+      <c r="BZ2" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="BS2" s="14" t="s">
+      <c r="CA2" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="BT2" s="14" t="s">
+      <c r="CB2" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="BU2" s="10" t="s">
+      <c r="CC2" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="CD2" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="CE2" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="CF2" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="CG2" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="CH2" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="CI2" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="CJ2" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="CK2" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="CL2" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="BV2" s="10" t="s">
+      <c r="CM2" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="BW2" s="10" t="s">
+      <c r="CN2" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="BX2" s="10" t="s">
+      <c r="CO2" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="BY2" s="10" t="s">
+      <c r="CP2" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="BZ2" s="10" t="s">
+      <c r="CQ2" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:78" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:95" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="15">
         <v>1</v>
       </c>
       <c r="B3" s="16"/>
       <c r="C3" s="15">
-        <f>A3+BV3-1</f>
+        <f>A3+CM3-1</f>
         <v>1</v>
       </c>
       <c r="D3" s="15">
         <v>1</v>
       </c>
       <c r="E3" s="15">
-        <f>D3+BV3-1</f>
+        <f>D3+CM3-1</f>
         <v>1</v>
       </c>
       <c r="F3" s="17" t="s">
@@ -1156,21 +1288,21 @@
       <c r="J3" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="K3" s="15">
+      <c r="K3" s="15"/>
+      <c r="L3" s="15">
         <v>3</v>
       </c>
-      <c r="L3" s="15">
+      <c r="M3" s="15">
         <v>13</v>
       </c>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15">
+      <c r="N3" s="15"/>
+      <c r="O3" s="15">
         <v>8</v>
       </c>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15">
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15">
         <v>15</v>
       </c>
-      <c r="Q3" s="15"/>
       <c r="R3" s="15"/>
       <c r="S3" s="15"/>
       <c r="T3" s="15"/>
@@ -1179,18 +1311,18 @@
       <c r="W3" s="15"/>
       <c r="X3" s="15"/>
       <c r="Y3" s="15"/>
-      <c r="Z3" s="15">
+      <c r="Z3" s="15"/>
+      <c r="AA3" s="15">
         <v>7</v>
       </c>
-      <c r="AA3" s="15"/>
-      <c r="AB3" s="15">
+      <c r="AB3" s="15"/>
+      <c r="AC3" s="15">
         <v>3</v>
       </c>
-      <c r="AC3" s="15"/>
-      <c r="AD3" s="15">
+      <c r="AD3" s="15"/>
+      <c r="AE3" s="15">
         <v>1</v>
       </c>
-      <c r="AE3" s="15"/>
       <c r="AF3" s="15"/>
       <c r="AG3" s="15"/>
       <c r="AH3" s="15"/>
@@ -1232,30 +1364,47 @@
       <c r="BR3" s="15"/>
       <c r="BS3" s="15"/>
       <c r="BT3" s="15"/>
-      <c r="BU3" s="1">
-        <f t="shared" ref="BU3:BU7" si="0">SUM(K3:AJ3)</f>
+      <c r="BU3" s="15"/>
+      <c r="BV3" s="15"/>
+      <c r="BW3" s="15"/>
+      <c r="BX3" s="15"/>
+      <c r="BY3" s="15"/>
+      <c r="BZ3" s="15"/>
+      <c r="CA3" s="15"/>
+      <c r="CB3" s="15"/>
+      <c r="CC3" s="15"/>
+      <c r="CD3" s="15"/>
+      <c r="CE3" s="15"/>
+      <c r="CF3" s="15"/>
+      <c r="CG3" s="15"/>
+      <c r="CH3" s="15"/>
+      <c r="CI3" s="15"/>
+      <c r="CJ3" s="15"/>
+      <c r="CK3" s="15"/>
+      <c r="CL3" s="1">
+        <f>SUM(L3:AK3)</f>
         <v>50</v>
       </c>
-      <c r="BV3" s="15">
+      <c r="CM3" s="15">
         <v>1</v>
       </c>
-      <c r="BW3" s="18">
-        <f>BU3*BV3</f>
+      <c r="CN3" s="18">
+        <f>CL3*CM3</f>
         <v>50</v>
       </c>
-      <c r="BX3" s="15">
-        <f>22*BV3</f>
+      <c r="CO3" s="15">
+        <f>22*CM3</f>
         <v>22</v>
       </c>
-      <c r="BY3" s="9">
-        <f>23*BV3</f>
+      <c r="CP3" s="9">
+        <f>23*CM3</f>
         <v>23</v>
       </c>
-      <c r="BZ3" s="19" t="s">
+      <c r="CQ3" s="19" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:78" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:95" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="15">
         <f>C3+1</f>
         <v>2</v>
@@ -1264,7 +1413,7 @@
         <v>31</v>
       </c>
       <c r="C4" s="15">
-        <f>A4+BV4-1</f>
+        <f>A4+CM4-1</f>
         <v>2</v>
       </c>
       <c r="D4" s="15">
@@ -1272,7 +1421,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="15">
-        <f>D4+BV4-1</f>
+        <f>D4+CM4-1</f>
         <v>2</v>
       </c>
       <c r="F4" s="17" t="s">
@@ -1297,22 +1446,22 @@
       <c r="O4" s="15"/>
       <c r="P4" s="15"/>
       <c r="Q4" s="15"/>
-      <c r="R4" s="15">
+      <c r="R4" s="15"/>
+      <c r="S4" s="15">
         <v>14</v>
       </c>
-      <c r="S4" s="15"/>
-      <c r="T4" s="15">
+      <c r="T4" s="15"/>
+      <c r="U4" s="15">
         <v>10</v>
       </c>
-      <c r="U4" s="15"/>
-      <c r="V4" s="15">
+      <c r="V4" s="15"/>
+      <c r="W4" s="15">
         <v>13</v>
       </c>
-      <c r="W4" s="15"/>
-      <c r="X4" s="15">
+      <c r="X4" s="15"/>
+      <c r="Y4" s="15">
         <v>8</v>
       </c>
-      <c r="Y4" s="15"/>
       <c r="Z4" s="15"/>
       <c r="AA4" s="15"/>
       <c r="AB4" s="15"/>
@@ -1360,39 +1509,56 @@
       <c r="BR4" s="15"/>
       <c r="BS4" s="15"/>
       <c r="BT4" s="15"/>
-      <c r="BU4" s="1">
-        <f t="shared" si="0"/>
+      <c r="BU4" s="15"/>
+      <c r="BV4" s="15"/>
+      <c r="BW4" s="15"/>
+      <c r="BX4" s="15"/>
+      <c r="BY4" s="15"/>
+      <c r="BZ4" s="15"/>
+      <c r="CA4" s="15"/>
+      <c r="CB4" s="15"/>
+      <c r="CC4" s="15"/>
+      <c r="CD4" s="15"/>
+      <c r="CE4" s="15"/>
+      <c r="CF4" s="15"/>
+      <c r="CG4" s="15"/>
+      <c r="CH4" s="15"/>
+      <c r="CI4" s="15"/>
+      <c r="CJ4" s="15"/>
+      <c r="CK4" s="15"/>
+      <c r="CL4" s="1">
+        <f>SUM(L4:AK4)</f>
         <v>45</v>
       </c>
-      <c r="BV4" s="15">
+      <c r="CM4" s="15">
         <v>1</v>
       </c>
-      <c r="BW4" s="18">
-        <f t="shared" ref="BW4:BW7" si="1">BU4*BV4</f>
+      <c r="CN4" s="18">
+        <f t="shared" ref="CN4:CN7" si="0">CL4*CM4</f>
         <v>45</v>
       </c>
-      <c r="BX4" s="15">
-        <f t="shared" ref="BX4:BX7" si="2">22*BV4</f>
+      <c r="CO4" s="15">
+        <f t="shared" ref="CO4:CO7" si="1">22*CM4</f>
         <v>22</v>
       </c>
-      <c r="BY4" s="9">
-        <f t="shared" ref="BY4:BY7" si="3">23*BV4</f>
+      <c r="CP4" s="9">
+        <f t="shared" ref="CP4:CP7" si="2">23*CM4</f>
         <v>23</v>
       </c>
-      <c r="BZ4" s="19" t="s">
+      <c r="CQ4" s="19" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:78" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:95" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="15">
-        <f t="shared" ref="A5:A7" si="4">C4+1</f>
+        <f t="shared" ref="A5:A7" si="3">C4+1</f>
         <v>3</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="15">
-        <f>A5+BV5-1</f>
+        <f>A5+CM5-1</f>
         <v>3</v>
       </c>
       <c r="D5" s="15">
@@ -1400,7 +1566,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="15">
-        <f>D5+BV5-1</f>
+        <f>D5+CM5-1</f>
         <v>3</v>
       </c>
       <c r="F5" s="17" t="s">
@@ -1418,37 +1584,37 @@
       <c r="J5" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="K5" s="15">
-        <v>5</v>
-      </c>
+      <c r="K5" s="15"/>
       <c r="L5" s="15">
         <v>5</v>
       </c>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15">
+      <c r="M5" s="15">
+        <v>5</v>
+      </c>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15">
         <v>4</v>
       </c>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15">
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15">
         <v>7</v>
       </c>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15">
+      <c r="R5" s="15"/>
+      <c r="S5" s="15">
         <v>8</v>
       </c>
-      <c r="S5" s="15"/>
-      <c r="T5" s="15">
+      <c r="T5" s="15"/>
+      <c r="U5" s="15">
         <v>4</v>
       </c>
-      <c r="U5" s="15"/>
-      <c r="V5" s="15">
+      <c r="V5" s="15"/>
+      <c r="W5" s="15">
         <v>6</v>
       </c>
-      <c r="W5" s="15"/>
-      <c r="X5" s="15">
+      <c r="X5" s="15"/>
+      <c r="Y5" s="15">
         <v>5</v>
       </c>
-      <c r="Y5" s="15"/>
       <c r="Z5" s="15"/>
       <c r="AA5" s="15"/>
       <c r="AB5" s="15"/>
@@ -1496,47 +1662,64 @@
       <c r="BR5" s="15"/>
       <c r="BS5" s="15"/>
       <c r="BT5" s="15"/>
-      <c r="BU5" s="1">
+      <c r="BU5" s="15"/>
+      <c r="BV5" s="15"/>
+      <c r="BW5" s="15"/>
+      <c r="BX5" s="15"/>
+      <c r="BY5" s="15"/>
+      <c r="BZ5" s="15"/>
+      <c r="CA5" s="15"/>
+      <c r="CB5" s="15"/>
+      <c r="CC5" s="15"/>
+      <c r="CD5" s="15"/>
+      <c r="CE5" s="15"/>
+      <c r="CF5" s="15"/>
+      <c r="CG5" s="15"/>
+      <c r="CH5" s="15"/>
+      <c r="CI5" s="15"/>
+      <c r="CJ5" s="15"/>
+      <c r="CK5" s="15"/>
+      <c r="CL5" s="1">
+        <f>SUM(L5:AK5)</f>
+        <v>44</v>
+      </c>
+      <c r="CM5" s="15">
+        <v>1</v>
+      </c>
+      <c r="CN5" s="18">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="BV5" s="15">
-        <v>1</v>
-      </c>
-      <c r="BW5" s="18">
+      <c r="CO5" s="15">
         <f t="shared" si="1"/>
-        <v>44</v>
-      </c>
-      <c r="BX5" s="15">
+        <v>22</v>
+      </c>
+      <c r="CP5" s="9">
         <f t="shared" si="2"/>
-        <v>22</v>
-      </c>
-      <c r="BY5" s="9">
+        <v>23</v>
+      </c>
+      <c r="CQ5" s="19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:95" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="15">
         <f t="shared" si="3"/>
-        <v>23</v>
-      </c>
-      <c r="BZ5" s="19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:78" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="15">
-        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>31</v>
       </c>
       <c r="C6" s="15">
-        <f>A6+BV6-1</f>
+        <f>A6+CM6-1</f>
         <v>4</v>
       </c>
       <c r="D6" s="15">
-        <f t="shared" ref="D6:D7" si="5">E5+1</f>
+        <f t="shared" ref="D6:D7" si="4">E5+1</f>
         <v>4</v>
       </c>
       <c r="E6" s="15">
-        <f>D6+BV6-1</f>
+        <f>D6+CM6-1</f>
         <v>4</v>
       </c>
       <c r="F6" s="17" t="s">
@@ -1554,21 +1737,21 @@
       <c r="J6" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="K6" s="15">
-        <v>10</v>
-      </c>
+      <c r="K6" s="15"/>
       <c r="L6" s="15">
         <v>10</v>
       </c>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15">
+      <c r="M6" s="15">
+        <v>10</v>
+      </c>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15">
         <v>7</v>
       </c>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15">
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15">
         <v>14</v>
       </c>
-      <c r="Q6" s="15"/>
       <c r="R6" s="15"/>
       <c r="S6" s="15"/>
       <c r="T6" s="15"/>
@@ -1624,47 +1807,64 @@
       <c r="BR6" s="15"/>
       <c r="BS6" s="15"/>
       <c r="BT6" s="15"/>
-      <c r="BU6" s="1">
+      <c r="BU6" s="15"/>
+      <c r="BV6" s="15"/>
+      <c r="BW6" s="15"/>
+      <c r="BX6" s="15"/>
+      <c r="BY6" s="15"/>
+      <c r="BZ6" s="15"/>
+      <c r="CA6" s="15"/>
+      <c r="CB6" s="15"/>
+      <c r="CC6" s="15"/>
+      <c r="CD6" s="15"/>
+      <c r="CE6" s="15"/>
+      <c r="CF6" s="15"/>
+      <c r="CG6" s="15"/>
+      <c r="CH6" s="15"/>
+      <c r="CI6" s="15"/>
+      <c r="CJ6" s="15"/>
+      <c r="CK6" s="15"/>
+      <c r="CL6" s="1">
+        <f>SUM(L6:AK6)</f>
+        <v>41</v>
+      </c>
+      <c r="CM6" s="15">
+        <v>1</v>
+      </c>
+      <c r="CN6" s="18">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="BV6" s="15">
-        <v>1</v>
-      </c>
-      <c r="BW6" s="18">
+      <c r="CO6" s="15">
         <f t="shared" si="1"/>
-        <v>41</v>
-      </c>
-      <c r="BX6" s="15">
+        <v>22</v>
+      </c>
+      <c r="CP6" s="9">
         <f t="shared" si="2"/>
-        <v>22</v>
-      </c>
-      <c r="BY6" s="9">
+        <v>23</v>
+      </c>
+      <c r="CQ6" s="19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:95" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="15">
         <f t="shared" si="3"/>
-        <v>23</v>
-      </c>
-      <c r="BZ6" s="19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:78" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="15">
+        <v>5</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="15">
+        <f>A7+CM7-1</f>
+        <v>5</v>
+      </c>
+      <c r="D7" s="15">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="15">
-        <f>A7+BV7-1</f>
-        <v>5</v>
-      </c>
-      <c r="D7" s="15">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
       <c r="E7" s="15">
-        <f>D7+BV7-1</f>
+        <f>D7+CM7-1</f>
         <v>5</v>
       </c>
       <c r="F7" s="17" t="s">
@@ -1689,18 +1889,18 @@
       <c r="O7" s="15"/>
       <c r="P7" s="15"/>
       <c r="Q7" s="15"/>
-      <c r="R7" s="15">
+      <c r="R7" s="15"/>
+      <c r="S7" s="15">
         <v>13</v>
       </c>
-      <c r="S7" s="15"/>
-      <c r="T7" s="15">
+      <c r="T7" s="15"/>
+      <c r="U7" s="15">
         <v>13</v>
       </c>
-      <c r="U7" s="15"/>
-      <c r="V7" s="15">
+      <c r="V7" s="15"/>
+      <c r="W7" s="15">
         <v>22</v>
       </c>
-      <c r="W7" s="15"/>
       <c r="X7" s="15"/>
       <c r="Y7" s="15"/>
       <c r="Z7" s="15"/>
@@ -1750,30 +1950,47 @@
       <c r="BR7" s="15"/>
       <c r="BS7" s="15"/>
       <c r="BT7" s="15"/>
-      <c r="BU7" s="1">
+      <c r="BU7" s="15"/>
+      <c r="BV7" s="15"/>
+      <c r="BW7" s="15"/>
+      <c r="BX7" s="15"/>
+      <c r="BY7" s="15"/>
+      <c r="BZ7" s="15"/>
+      <c r="CA7" s="15"/>
+      <c r="CB7" s="15"/>
+      <c r="CC7" s="15"/>
+      <c r="CD7" s="15"/>
+      <c r="CE7" s="15"/>
+      <c r="CF7" s="15"/>
+      <c r="CG7" s="15"/>
+      <c r="CH7" s="15"/>
+      <c r="CI7" s="15"/>
+      <c r="CJ7" s="15"/>
+      <c r="CK7" s="15"/>
+      <c r="CL7" s="1">
+        <f>SUM(L7:AK7)</f>
+        <v>48</v>
+      </c>
+      <c r="CM7" s="15">
+        <v>1</v>
+      </c>
+      <c r="CN7" s="18">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="BV7" s="15">
-        <v>1</v>
-      </c>
-      <c r="BW7" s="18">
+      <c r="CO7" s="15">
         <f t="shared" si="1"/>
-        <v>48</v>
-      </c>
-      <c r="BX7" s="15">
+        <v>22</v>
+      </c>
+      <c r="CP7" s="9">
         <f t="shared" si="2"/>
-        <v>22</v>
-      </c>
-      <c r="BY7" s="9">
-        <f t="shared" si="3"/>
         <v>23</v>
       </c>
-      <c r="BZ7" s="19" t="s">
+      <c r="CQ7" s="19" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:95" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1784,8 +2001,9 @@
       <c r="H8" s="3"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:95" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1796,8 +2014,9 @@
       <c r="H9" s="3"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:95" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1808,8 +2027,9 @@
       <c r="H10" s="3"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:95" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="4"/>
@@ -1820,6 +2040,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>